<commit_message>
build a apresentar ao negócio
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://groupecgi-my.sharepoint.com/personal/brunofilipe_lobo_cgi_com/Documents/Code/realvidaseguros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="11_F25DC773A252ABDACC1048DA19DC7D545ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F544B05B-760E-4CD6-9EC7-D69BA12EEA73}"/>
+  <xr:revisionPtr revIDLastSave="503" documentId="11_F25DC773A252ABDACC1048DA19DC7D545ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA087276-2E31-4823-9340-96DC1F52FE75}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32460" yWindow="825" windowWidth="23175" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="114">
   <si>
     <t>name</t>
   </si>
@@ -325,24 +325,6 @@
     <t>Tratamento RPA</t>
   </si>
   <si>
-    <t>TratamentoManualClickToCall</t>
-  </si>
-  <si>
-    <t>Tratamento Manual - Recorrências</t>
-  </si>
-  <si>
-    <t>TratamentoManualRecorrencias</t>
-  </si>
-  <si>
-    <t>Tratamento Manual - Contacto Click to Call</t>
-  </si>
-  <si>
-    <t>Nome Pasta a mover emails de Regra Recorrência</t>
-  </si>
-  <si>
-    <t>Nome Pasta a mover emails de Regra Click to Call</t>
-  </si>
-  <si>
     <t>Emails de excepcao onde o dispatcher discarta automaticamente o email</t>
   </si>
   <si>
@@ -373,12 +355,6 @@
     <t>IntelligentProcessAutomationNLP\Automation\RegrasEmails.xlsx</t>
   </si>
   <si>
-    <t>IntelligentProcessAutomationNLP\Automation\intencoes.xlsx</t>
-  </si>
-  <si>
-    <t>IntelligentProcessAutomationNLP\Automation\classificacaoapolices.xlsx</t>
-  </si>
-  <si>
     <t>IntelligentProcessAutomationNLP/ModelNLP/</t>
   </si>
   <si>
@@ -404,9 +380,6 @@
   </si>
   <si>
     <t>EmailTratamentoManualMove</t>
-  </si>
-  <si>
-    <t>Tratamento RNA</t>
   </si>
   <si>
     <t>Nome da pasta a mover os emails depois de Erro ao Processar</t>
@@ -469,6 +442,53 @@
     <t>Boa tarde,
 O processamento do RPA terminou: [E]
 (Email enviado automaticamente, não responder)</t>
+  </si>
+  <si>
+    <t>EM02_To</t>
+  </si>
+  <si>
+    <t>EM02_Subject</t>
+  </si>
+  <si>
+    <t>RPA Pedidos de Clientes por Email – Status Processamento</t>
+  </si>
+  <si>
+    <t>EM02_Body</t>
+  </si>
+  <si>
+    <t>Tratamento Manual</t>
+  </si>
+  <si>
+    <t>Boa tarde,
+O processamento do RPA terminou.
+Pedidos Processados: [A]
+Pedidos Tratamento RPA: [B]
+•	Reforços apólices financeiras (ID/Label: 0): [D]
+•	Atualização dados pessoais:
+o	Morada, telefone, telemóvel e email (ID/Label: 1): [E]
+o	Data de nascimento, nome, nif, sexo (ID/Label: 2): [F]
+•	Atualização de capital da apólice (ID/Label: 3): [G]
+•	Pedido de resgate de apólice financeira (ID/Label: 5) : [H]
+•	Acesso à Área Reservada de Clientes (MyRealVida) (ID/Label: 6) : [I]
+•	Alteração de Iban de débito (ID/Label: 7) : [J]
+•	Pedido de anulação de apólices Universo (ID/Label: 8) : [K]
+•	Participação de sinistros Acidentes Pessoais (ID/Label: 9): [L]
+•	Participação de sinistros Vida Risco (ID/Label: 10): [M]
+•	Contacto não identificado: [N]
+Pedidos Tratamento RNA: [C]
+(Email enviado automaticamente, não responder)</t>
+  </si>
+  <si>
+    <t>IntelligentProcessAutomationNLP\Automation\Intencoes.xlsx</t>
+  </si>
+  <si>
+    <t>IntelligentProcessAutomationNLP\Automation\ClassificacaoApolices.xlsx</t>
+  </si>
+  <si>
+    <t>NÃO modificar</t>
+  </si>
+  <si>
+    <t>ChromePath</t>
   </si>
 </sst>
 </file>
@@ -496,7 +516,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,12 +535,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -534,15 +548,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,242 +860,245 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="1" t="b">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
+      <c r="A23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1091,7 +1106,7 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -1102,7 +1117,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
@@ -1110,128 +1125,119 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26">
-        <v>0.1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>0.2</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,39 +1245,55 @@
         <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
-      </c>
-      <c r="B40" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build com alterações a pedido do cliente
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://groupecgi-my.sharepoint.com/personal/brunofilipe_lobo_cgi_com/Documents/Code/realvidaseguros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="11_F25DC773A252ABDACC1048DA19DC7D545ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA087276-2E31-4823-9340-96DC1F52FE75}"/>
+  <xr:revisionPtr revIDLastSave="519" documentId="11_F25DC773A252ABDACC1048DA19DC7D545ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47726D1C-9087-46BC-AA80-ED076591DC38}"/>
   <bookViews>
-    <workbookView xWindow="32460" yWindow="825" windowWidth="23175" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4305" yWindow="-16320" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="119">
   <si>
     <t>name</t>
   </si>
@@ -398,9 +398,6 @@
   </si>
   <si>
     <t>Teste_Dispatcher_NLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE se for Teste Output NLP Else "FALSE" </t>
   </si>
   <si>
     <t>Pedidos_Teste</t>
@@ -489,6 +486,98 @@
   </si>
   <si>
     <t>ChromePath</t>
+  </si>
+  <si>
+    <t>ClienteSemEmailEmail</t>
+  </si>
+  <si>
+    <t>x@x.pt</t>
+  </si>
+  <si>
+    <t>TRUE se for Teste Output NLP Else "FALSE"  (Default é False)</t>
+  </si>
+  <si>
+    <r>
+      <t>C:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rogram Files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>oogle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>hrome\Application</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>hrome.exe</t>
+    </r>
+  </si>
+  <si>
+    <t>pathOutput</t>
+  </si>
+  <si>
+    <t>Output\</t>
   </si>
 </sst>
 </file>
@@ -548,12 +637,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -835,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:B33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,15 +970,15 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
         <v>85</v>
@@ -894,10 +986,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>86</v>
@@ -905,10 +997,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>87</v>
@@ -966,7 +1058,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,210 +1107,207 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>97</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29">
-        <v>0.2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>38</v>
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" t="s">
-        <v>75</v>
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>0.1</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
         <v>58</v>
@@ -1226,74 +1315,96 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>104</v>
       </c>
-      <c r="B42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B45" t="s">
         <v>105</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="315" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>109</v>
+      <c r="B46" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build Final (Ajustes nos logs)
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://groupecgi-my.sharepoint.com/personal/brunofilipe_lobo_cgi_com/Documents/Code/realvidaseguros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="539" documentId="11_F25DC773A252ABDACC1048DA19DC7D545ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D4677EA-6687-4FB6-B6B2-5029D794E9B7}"/>
+  <xr:revisionPtr revIDLastSave="541" documentId="11_F25DC773A252ABDACC1048DA19DC7D545ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F97C12E2-3B8C-4CBD-9099-370A11EAE0FF}"/>
   <bookViews>
-    <workbookView xWindow="-4305" yWindow="-16320" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,22 +577,22 @@
     <t>pathOutput</t>
   </si>
   <si>
+    <t>pathLogs</t>
+  </si>
+  <si>
+    <t>SLA_Performer</t>
+  </si>
+  <si>
+    <t>SLA_Dispatcher</t>
+  </si>
+  <si>
+    <t>SLA Definido em Horas Dispatcher</t>
+  </si>
+  <si>
+    <t>SLA Definido em Horas Performer</t>
+  </si>
+  <si>
     <t>Output\</t>
-  </si>
-  <si>
-    <t>pathLogs</t>
-  </si>
-  <si>
-    <t>SLA_Performer</t>
-  </si>
-  <si>
-    <t>SLA_Dispatcher</t>
-  </si>
-  <si>
-    <t>SLA Definido em Horas Dispatcher</t>
-  </si>
-  <si>
-    <t>SLA Definido em Horas Performer</t>
   </si>
 </sst>
 </file>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,24 +1096,24 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B13" s="5">
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="5">
         <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1400,12 +1400,12 @@
         <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>